<commit_message>
updates a missing room, fixes overlapping in another room
</commit_message>
<xml_diff>
--- a/ROOMS.xlsx
+++ b/ROOMS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pewpewded/Desktop/excel-rooms-converter/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{901F5752-7D3B-6C45-92DD-DB1ABD661AAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF80A8A0-483D-024A-9AC4-CA88BE75DEBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1026" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="371">
   <si>
     <t>Room:</t>
   </si>
@@ -1130,6 +1130,9 @@
   </si>
   <si>
     <t>97 PHY 203 | 126 PHY 203</t>
+  </si>
+  <si>
+    <t>G120</t>
   </si>
 </sst>
 </file>
@@ -1953,8 +1956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H510"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" topLeftCell="A172" zoomScale="107" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J194" sqref="J194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4453,8 +4456,12 @@
       </c>
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B190"/>
-      <c r="C190"/>
+      <c r="B190" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C190" s="1" t="s">
+        <v>370</v>
+      </c>
       <c r="D190"/>
       <c r="E190"/>
       <c r="F190"/>

</xml_diff>